<commit_message>
Adapt pearson corre into kafka @clin1
</commit_message>
<xml_diff>
--- a/scripts/inputs_qserver_kafka_v2.xlsx
+++ b/scripts/inputs_qserver_kafka_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="kafka_1LL09" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="184">
   <si>
     <t xml:space="preserve">Input parameters for data process in kafka</t>
   </si>
@@ -434,6 +434,24 @@
   </si>
   <si>
     <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/agent_data/Cl_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pearson_pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simulated_gr_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/pearson_multi_phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simulated_gr_fn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CsBr.gr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cs4PbBr6.gr</t>
   </si>
   <si>
     <t xml:space="preserve">CsPb(oleate)3_30mM_20240216</t>
@@ -933,14 +951,14 @@
       <selection pane="topLeft" activeCell="H35" activeCellId="0" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1536,7 +1554,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.03125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -1547,12 +1565,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -1566,7 +1584,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1667,13 +1685,13 @@
         <v>76</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>123</v>
@@ -1772,7 +1790,7 @@
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -1812,7 +1830,7 @@
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>36</v>
@@ -2260,11 +2278,11 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -3046,7 +3064,7 @@
       <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.03125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -3611,20 +3629,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E44" activeCellId="0" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6796875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6953125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3950,58 +3968,90 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>49</v>
+        <v>135</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>136</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
+        <v>138</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B52" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C52" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D52" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E52" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="F52" s="0" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B44" r:id="rId1" display="https://tiled.nsls2.bnl.gov/api/v1/metadata/xpd/sandbox"/>
+    <hyperlink ref="B49" r:id="rId1" display="https://tiled.nsls2.bnl.gov/api/v1/metadata/xpd/sandbox"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4024,7 +4074,7 @@
       <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.03125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -4136,13 +4186,13 @@
         <v>76</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>81</v>
@@ -4493,14 +4543,14 @@
       <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6796875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6953125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4521,7 +4571,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4891,30 +4941,30 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.03125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="78.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="78.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4922,7 +4972,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4930,7 +4980,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4938,7 +4988,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4946,7 +4996,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4954,7 +5004,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4962,7 +5012,7 @@
         <v>70</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4970,7 +5020,7 @@
         <v>76</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4978,7 +5028,7 @@
         <v>82</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4986,7 +5036,7 @@
         <v>85</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4994,7 +5044,7 @@
         <v>86</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5002,7 +5052,7 @@
         <v>92</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5010,15 +5060,15 @@
         <v>103</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5026,7 +5076,7 @@
         <v>105</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5034,7 +5084,7 @@
         <v>114</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5042,7 +5092,7 @@
         <v>114</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5050,7 +5100,7 @@
         <v>114</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5058,7 +5108,7 @@
         <v>113</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5066,7 +5116,7 @@
         <v>113</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5074,7 +5124,7 @@
         <v>113</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -5099,10 +5149,10 @@
       <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.03125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="78.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="78.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.66"/>
   </cols>
   <sheetData>
@@ -5111,15 +5161,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5127,7 +5177,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5135,7 +5185,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5143,7 +5193,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5151,7 +5201,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5159,7 +5209,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5167,12 +5217,12 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5180,7 +5230,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5188,7 +5238,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5196,12 +5246,12 @@
         <v>17</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5209,7 +5259,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5217,7 +5267,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5225,12 +5275,12 @@
         <v>20</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5238,7 +5288,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5246,7 +5296,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5254,12 +5304,12 @@
         <v>24</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5267,7 +5317,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5387,7 +5437,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.03125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>
@@ -5397,12 +5447,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -5413,7 +5463,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5512,13 +5562,13 @@
         <v>76</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5568,10 +5618,10 @@
         <v>92</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5587,7 +5637,7 @@
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>50</v>
@@ -5596,7 +5646,7 @@
         <v>101</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>300</v>
@@ -5615,13 +5665,13 @@
         <v>114</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5629,13 +5679,13 @@
         <v>114</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5643,13 +5693,13 @@
         <v>114</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5657,13 +5707,13 @@
         <v>114</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>